<commit_message>
RDM-6557: Updated the email ID's for test data.
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_BEFTA_JURISDICTION1.xlsx
+++ b/src/aat/resources/CCD_BEFTA_JURISDICTION1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/462450/IdeaProjects/ccd-docker/bin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC4972D-B599-504F-95CD-815123DB72EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F8422E-94AB-E440-9FB9-0916DEF6FC92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28140" windowHeight="16420" tabRatio="823" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -633,7 +633,7 @@
     <t>BEFTA Case Type 1 1</t>
   </si>
   <si>
-    <t>befta_caseworker1@beftajurisdiction1.gmail.com</t>
+    <t>befta_caseworker_1@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -922,6 +922,7 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2541,7 +2542,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2608,7 +2609,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" xr:uid="{E2948D50-B85B-874E-AE33-6B0162BDF2ED}"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{8B926E64-430E-6145-802C-ABE2E2DD536B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
RDM-6557: Updated the user creation.
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_BEFTA_JURISDICTION1.xlsx
+++ b/src/aat/resources/CCD_BEFTA_JURISDICTION1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/462450/IdeaProjects/ccd-docker/bin/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/462450/IdeaProjects/ccd-data-store-api/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F8422E-94AB-E440-9FB9-0916DEF6FC92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101AAF0D-C58E-A243-8860-7D385F8FA4FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28140" windowHeight="16420" tabRatio="823" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -633,7 +633,7 @@
     <t>BEFTA Case Type 1 1</t>
   </si>
   <si>
-    <t>befta_caseworker_1@gmail.com</t>
+    <t>befta.caseworker.1@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2542,7 +2542,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
RDM-6385: Updated case type in CCD_BEFTA_JURISDICTION1.xlsx file.
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_BEFTA_JURISDICTION1.xlsx
+++ b/src/aat/resources/CCD_BEFTA_JURISDICTION1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/462450/IdeaProjects/ccd-data-store-api/src/aat/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sivakanukollu/github/MOJ/ccd-data-store-api/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101AAF0D-C58E-A243-8860-7D385F8FA4FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0763617F-8080-7143-86ED-B424606C3913}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28140" windowHeight="16420" tabRatio="823" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-11560" yWindow="-26880" windowWidth="50900" windowHeight="26880" tabRatio="823" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="194">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -634,6 +634,15 @@
   </si>
   <si>
     <t>befta.caseworker.1@gmail.com</t>
+  </si>
+  <si>
+    <t>CASE_TYPE_WITH_NO_CASES</t>
+  </si>
+  <si>
+    <t>DO NOT CREATE CASES FOR THIS CASE TYPE</t>
+  </si>
+  <si>
+    <t>Create a case of type CASE_TYPE_WITH_NO_CASES</t>
   </si>
 </sst>
 </file>
@@ -1595,10 +1604,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+      <selection activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1699,15 +1708,51 @@
         <v>2</v>
       </c>
     </row>
+    <row r="6" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="23">
+        <v>43466</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="F6" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="23">
+        <v>43466</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="F7" s="21">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F5" xr:uid="{00000000-0002-0000-0900-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F7" xr:uid="{00000000-0002-0000-0900-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A5" xr:uid="{00000000-0002-0000-0900-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A7" xr:uid="{00000000-0002-0000-0900-000002000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B5" xr:uid="{00000000-0002-0000-0900-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B7" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -1715,12 +1760,18 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{00000000-0002-0000-0900-000004000000}">
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$9</xm:f>
           </x14:formula1>
           <xm:sqref>D4:D5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{1BAD95F9-41BA-5842-BA71-6EE162088107}">
+          <x14:formula1>
+            <xm:f>'/Users/sivakanukollu/github/MOJ/ccd-data-store-api/src/aat/resources/[CCD_BEFTA_JURISDICTION4.xlsx]CaseField'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>D6:D7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1733,10 +1784,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:F4"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1820,15 +1871,33 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B5" s="26"/>
+      <c r="C5" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="F5" s="21">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4" xr:uid="{00000000-0002-0000-0A00-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A5" xr:uid="{00000000-0002-0000-0A00-000000000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4" xr:uid="{00000000-0002-0000-0A00-000002000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F5" xr:uid="{00000000-0002-0000-0A00-000002000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B4" xr:uid="{00000000-0002-0000-0A00-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B4:B5" xr:uid="{00000000-0002-0000-0A00-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -1836,12 +1905,18 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{00000000-0002-0000-0A00-000003000000}">
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$9</xm:f>
           </x14:formula1>
           <xm:sqref>D4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{8F00E64D-9BA3-5E44-B5C4-8D0ED00EF488}">
+          <x14:formula1>
+            <xm:f>'/Users/sivakanukollu/github/MOJ/ccd-data-store-api/src/aat/resources/[CCD_BEFTA_JURISDICTION4.xlsx]CaseField'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1854,10 +1929,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1958,15 +2033,51 @@
         <v>2</v>
       </c>
     </row>
+    <row r="6" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="23">
+        <v>43466</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="F6" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="23">
+        <v>43466</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="F7" s="21">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F5" xr:uid="{00000000-0002-0000-0B00-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F7" xr:uid="{00000000-0002-0000-0B00-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A5" xr:uid="{00000000-0002-0000-0B00-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A7" xr:uid="{00000000-0002-0000-0B00-000002000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B5" xr:uid="{00000000-0002-0000-0B00-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B7" xr:uid="{00000000-0002-0000-0B00-000000000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -1974,12 +2085,18 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{00000000-0002-0000-0B00-000004000000}">
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$9</xm:f>
           </x14:formula1>
           <xm:sqref>D4:D5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{53E8C99B-8925-A444-8303-0B51961AB1C2}">
+          <x14:formula1>
+            <xm:f>'/Users/sivakanukollu/github/MOJ/ccd-data-store-api/src/aat/resources/[CCD_BEFTA_JURISDICTION4.xlsx]CaseField'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>D6:D7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1995,7 +2112,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="A10" sqref="A10:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2246,64 +2363,166 @@
       </c>
     </row>
     <row r="10" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="27"/>
+      <c r="A10" s="27">
+        <v>43466</v>
+      </c>
       <c r="B10" s="27"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="28"/>
+      <c r="C10" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="G10" s="28">
+        <v>1</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="I10" s="28">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="27"/>
+      <c r="A11" s="27">
+        <v>43466</v>
+      </c>
       <c r="B11" s="27"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="28"/>
+      <c r="C11" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="G11" s="28">
+        <v>1</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="I11" s="28">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="27"/>
+      <c r="A12" s="27">
+        <v>43466</v>
+      </c>
       <c r="B12" s="27"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="28"/>
+      <c r="C12" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="G12" s="28">
+        <v>1</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="I12" s="28">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="27"/>
+      <c r="A13" s="27">
+        <v>43466</v>
+      </c>
       <c r="B13" s="27"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="28"/>
+      <c r="C13" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="G13" s="28">
+        <v>1</v>
+      </c>
+      <c r="H13" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="I13" s="28">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="27"/>
+      <c r="A14" s="27">
+        <v>43466</v>
+      </c>
       <c r="B14" s="27"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="28"/>
+      <c r="C14" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="G14" s="28">
+        <v>1</v>
+      </c>
+      <c r="H14" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="I14" s="28">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="27"/>
+      <c r="A15" s="27">
+        <v>43466</v>
+      </c>
       <c r="B15" s="27"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="28"/>
+      <c r="C15" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="G15" s="28">
+        <v>2</v>
+      </c>
+      <c r="H15" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="I15" s="28">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
@@ -2517,7 +2736,7 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G36 I4:I36" xr:uid="{00000000-0002-0000-0C00-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="I4:I36 G4:G36" xr:uid="{00000000-0002-0000-0C00-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A36" xr:uid="{00000000-0002-0000-0C00-000002000000}">
@@ -2541,8 +2760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2626,7 +2845,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2714,10 +2933,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="A7" sqref="A7:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2837,6 +3056,60 @@
         <v>120</v>
       </c>
     </row>
+    <row r="7" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="59">
+        <v>43466</v>
+      </c>
+      <c r="B7" s="53"/>
+      <c r="C7" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="E7" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F7" s="73" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="59">
+        <v>43466</v>
+      </c>
+      <c r="B8" s="53"/>
+      <c r="C8" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="E8" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" s="73" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="59">
+        <v>43466</v>
+      </c>
+      <c r="B9" s="53"/>
+      <c r="C9" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F9" s="73" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2853,7 +3126,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A10" sqref="A10:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3020,34 +3293,106 @@
       </c>
     </row>
     <row r="10" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="72"/>
-      <c r="D10" s="42"/>
-      <c r="F10" s="24"/>
+      <c r="A10" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E10" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="11" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="72"/>
-      <c r="D11" s="42"/>
-      <c r="F11" s="24"/>
+      <c r="A11" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="E11" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="12" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="72"/>
-      <c r="D12" s="42"/>
-      <c r="F12" s="24"/>
+      <c r="A12" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="13" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="72"/>
-      <c r="D13" s="42"/>
-      <c r="F13" s="24"/>
+      <c r="A13" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E13" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="14" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="72"/>
-      <c r="D14" s="42"/>
-      <c r="F14" s="24"/>
+      <c r="A14" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="E14" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="15" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="72"/>
-      <c r="D15" s="42"/>
-      <c r="F15" s="24"/>
+      <c r="A15" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="E15" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>120</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3065,7 +3410,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A10" sqref="A10:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3231,38 +3576,106 @@
       </c>
     </row>
     <row r="10" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="72"/>
-      <c r="D10" s="42"/>
-      <c r="E10"/>
-      <c r="F10" s="24"/>
+      <c r="A10" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="11" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="72"/>
-      <c r="D11" s="42"/>
-      <c r="F11" s="24"/>
+      <c r="A11" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="12" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="72"/>
-      <c r="D12" s="42"/>
-      <c r="E12"/>
-      <c r="F12" s="24"/>
+      <c r="A12" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="13" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="72"/>
-      <c r="D13" s="42"/>
-      <c r="E13"/>
-      <c r="F13" s="24"/>
+      <c r="A13" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="E13" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="14" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="72"/>
-      <c r="D14" s="42"/>
-      <c r="E14"/>
-      <c r="F14" s="24"/>
+      <c r="A14" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="E14" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="15" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="72"/>
-      <c r="D15" s="24"/>
-      <c r="F15" s="24"/>
+      <c r="A15" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="E15" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="72"/>
@@ -3390,8 +3803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FBCB2E-F376-5E45-8D3D-BA39DB091F6A}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3496,7 +3909,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3505,7 +3918,7 @@
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.83203125" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" customWidth="1"/>
     <col min="8" max="8" width="16.33203125" customWidth="1"/>
@@ -3606,15 +4019,36 @@
         <v>113</v>
       </c>
     </row>
+    <row r="5" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>193</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
     <row r="26" spans="10:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J26" s="85"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" xWindow="279" yWindow="381" count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4" xr:uid="{00000000-0002-0000-0100-000000000000}">
+  <dataValidations xWindow="279" yWindow="381" count="2">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A5" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B5" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -3630,10 +4064,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3919,12 +4353,186 @@
         <v>113</v>
       </c>
     </row>
+    <row r="10" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="G12" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="E13" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="G13" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="E14" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="F14" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="G14" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="E15" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="F15" s="42" t="s">
+        <v>147</v>
+      </c>
+      <c r="G15" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A9" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A15" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B15" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -3943,7 +4551,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4317,7 +4925,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C11" sqref="C11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4442,28 +5050,61 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="13"/>
+      <c r="A7" s="13">
+        <v>43466</v>
+      </c>
       <c r="B7" s="13"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
+      <c r="C7" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="E7" s="42" t="s">
+        <v>148</v>
+      </c>
       <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
+      <c r="G7" s="28">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="13"/>
+      <c r="A8" s="13">
+        <v>43466</v>
+      </c>
       <c r="B8" s="13"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
+      <c r="C8" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="E8" s="42" t="s">
+        <v>152</v>
+      </c>
       <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
+      <c r="G8" s="28">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="13"/>
+      <c r="A9" s="13">
+        <v>43466</v>
+      </c>
       <c r="B9" s="13"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
+      <c r="C9" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="42" t="s">
+        <v>151</v>
+      </c>
       <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
+      <c r="G9" s="28">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -4492,7 +5133,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D9"/>
+      <selection activeCell="A10" sqref="A10:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4852,106 +5493,224 @@
       </c>
     </row>
     <row r="10" spans="1:17" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="13"/>
+      <c r="A10" s="13">
+        <v>43466</v>
+      </c>
       <c r="B10" s="13"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
+      <c r="C10" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E10" s="42" t="s">
+        <v>155</v>
+      </c>
       <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
+      <c r="G10" s="28">
+        <v>1</v>
+      </c>
       <c r="H10" s="28"/>
-      <c r="I10" s="42"/>
+      <c r="I10" s="42" t="s">
+        <v>149</v>
+      </c>
       <c r="J10" s="30"/>
       <c r="K10" s="30"/>
       <c r="L10" s="30"/>
       <c r="M10" s="30"/>
       <c r="N10" s="30"/>
       <c r="O10" s="30"/>
-      <c r="Q10" s="24"/>
+      <c r="P10" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q10" s="24" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="11" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="13"/>
+      <c r="A11" s="13">
+        <v>43466</v>
+      </c>
       <c r="B11" s="13"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
+      <c r="C11" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>157</v>
+      </c>
       <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="42"/>
+      <c r="G11" s="28">
+        <v>2</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="I11" s="42" t="s">
+        <v>150</v>
+      </c>
       <c r="J11" s="30"/>
       <c r="K11" s="30"/>
       <c r="L11" s="30"/>
       <c r="M11" s="30"/>
       <c r="N11" s="30"/>
       <c r="O11" s="30"/>
-      <c r="Q11" s="24"/>
+      <c r="P11" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q11" s="24" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="12" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="13"/>
+      <c r="A12" s="13">
+        <v>43466</v>
+      </c>
       <c r="B12" s="13"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
+      <c r="C12" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" s="42" t="s">
+        <v>159</v>
+      </c>
       <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
+      <c r="G12" s="28">
+        <v>3</v>
+      </c>
+      <c r="H12" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="I12" s="42" t="s">
+        <v>149</v>
+      </c>
       <c r="J12" s="30"/>
       <c r="K12" s="30"/>
       <c r="L12" s="30"/>
       <c r="M12" s="30"/>
       <c r="N12" s="30"/>
       <c r="O12" s="30"/>
-      <c r="Q12" s="24"/>
+      <c r="P12" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q12" s="24" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="13" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="13"/>
+      <c r="A13" s="13">
+        <v>43466</v>
+      </c>
       <c r="B13" s="13"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
+      <c r="C13" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E13" s="42" t="s">
+        <v>161</v>
+      </c>
       <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
+      <c r="G13" s="28">
+        <v>4</v>
+      </c>
+      <c r="H13" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="I13" s="42" t="s">
+        <v>153</v>
+      </c>
       <c r="J13" s="30"/>
       <c r="K13" s="30"/>
       <c r="L13" s="30"/>
       <c r="M13" s="30"/>
       <c r="N13" s="30"/>
       <c r="O13" s="30"/>
-      <c r="Q13" s="24"/>
+      <c r="P13" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q13" s="24" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="14" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="13"/>
+      <c r="A14" s="13">
+        <v>43466</v>
+      </c>
       <c r="B14" s="13"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
+      <c r="C14" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="E14" s="42" t="s">
+        <v>163</v>
+      </c>
       <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
+      <c r="G14" s="28">
+        <v>5</v>
+      </c>
+      <c r="H14" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="I14" s="42" t="s">
+        <v>164</v>
+      </c>
       <c r="J14" s="30"/>
       <c r="K14" s="30"/>
       <c r="L14" s="30"/>
       <c r="M14" s="30"/>
       <c r="N14" s="30"/>
       <c r="O14" s="30"/>
-      <c r="Q14" s="24"/>
+      <c r="P14" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q14" s="24" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="15" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="13"/>
+      <c r="A15" s="13">
+        <v>43466</v>
+      </c>
       <c r="B15" s="13"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
+      <c r="C15" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="E15" s="42" t="s">
+        <v>171</v>
+      </c>
       <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
+      <c r="G15" s="28">
+        <v>6</v>
+      </c>
+      <c r="H15" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="I15" s="42" t="s">
+        <v>164</v>
+      </c>
       <c r="J15" s="30"/>
       <c r="K15" s="30"/>
       <c r="L15" s="30"/>
       <c r="M15" s="30"/>
       <c r="N15" s="30"/>
       <c r="O15" s="30"/>
-      <c r="Q15" s="24"/>
+      <c r="P15" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q15" s="24" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -4977,10 +5736,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5778,12 +6537,678 @@
         <v>26</v>
       </c>
     </row>
+    <row r="22" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B22" s="13"/>
+      <c r="C22" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D22" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="F22" s="28">
+        <v>1</v>
+      </c>
+      <c r="G22" s="28"/>
+      <c r="H22" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="I22" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="J22" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="K22" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="L22" s="14">
+        <v>1</v>
+      </c>
+      <c r="O22" s="24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B23" s="13"/>
+      <c r="C23" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D23" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="F23" s="28">
+        <v>2</v>
+      </c>
+      <c r="G23" s="28"/>
+      <c r="H23" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="I23" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="J23" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="K23" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="L23" s="14">
+        <v>1</v>
+      </c>
+      <c r="O23" s="24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B24" s="13"/>
+      <c r="C24" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="F24" s="28">
+        <v>3</v>
+      </c>
+      <c r="G24" s="28"/>
+      <c r="H24" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="I24" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="J24" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="K24" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="L24" s="14">
+        <v>1</v>
+      </c>
+      <c r="O24" s="24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D25" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E25" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="F25" s="28">
+        <v>4</v>
+      </c>
+      <c r="G25" s="28"/>
+      <c r="H25" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="I25" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="J25" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="K25" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="L25" s="14">
+        <v>1</v>
+      </c>
+      <c r="O25" s="24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D26" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E26" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="F26" s="28">
+        <v>5</v>
+      </c>
+      <c r="G26" s="28"/>
+      <c r="H26" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="I26" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="J26" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="K26" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="L26" s="14">
+        <v>1</v>
+      </c>
+      <c r="O26" s="24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E27" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F27" s="28">
+        <v>1</v>
+      </c>
+      <c r="G27" s="28"/>
+      <c r="H27" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="I27" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="J27" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="K27" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="L27" s="14">
+        <v>2</v>
+      </c>
+      <c r="O27" s="24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B28" s="13"/>
+      <c r="C28" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D28" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="F28" s="28">
+        <v>1</v>
+      </c>
+      <c r="G28" s="28"/>
+      <c r="H28" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="I28" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="J28" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="K28" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="L28" s="14">
+        <v>1</v>
+      </c>
+      <c r="O28" s="24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B29" s="13"/>
+      <c r="C29" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D29" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="F29" s="28">
+        <v>2</v>
+      </c>
+      <c r="G29" s="28"/>
+      <c r="H29" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="I29" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="J29" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="K29" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="L29" s="14">
+        <v>1</v>
+      </c>
+      <c r="O29" s="24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B30" s="13"/>
+      <c r="C30" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D30" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="F30" s="28">
+        <v>3</v>
+      </c>
+      <c r="G30" s="28"/>
+      <c r="H30" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="I30" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="J30" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="K30" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="L30" s="14">
+        <v>1</v>
+      </c>
+      <c r="O30" s="24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B31" s="13"/>
+      <c r="C31" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D31" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="E31" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="F31" s="28">
+        <v>4</v>
+      </c>
+      <c r="G31" s="28"/>
+      <c r="H31" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="I31" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="J31" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="K31" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="L31" s="14">
+        <v>1</v>
+      </c>
+      <c r="O31" s="24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B32" s="13"/>
+      <c r="C32" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D32" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="E32" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="F32" s="28">
+        <v>5</v>
+      </c>
+      <c r="G32" s="28"/>
+      <c r="H32" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="I32" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="J32" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="K32" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="L32" s="14">
+        <v>1</v>
+      </c>
+      <c r="O32" s="24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B33" s="13"/>
+      <c r="C33" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D33" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="E33" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F33" s="28">
+        <v>1</v>
+      </c>
+      <c r="G33" s="28"/>
+      <c r="H33" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="I33" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="J33" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="K33" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="L33" s="14">
+        <v>2</v>
+      </c>
+      <c r="O33" s="24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B34" s="13"/>
+      <c r="C34" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D34" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="F34" s="28">
+        <v>1</v>
+      </c>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="I34" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="J34" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="K34" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="L34" s="14">
+        <v>1</v>
+      </c>
+      <c r="O34" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B35" s="13"/>
+      <c r="C35" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D35" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="F35" s="28">
+        <v>2</v>
+      </c>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="I35" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="J35" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="K35" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="L35" s="14">
+        <v>1</v>
+      </c>
+      <c r="O35" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B36" s="13"/>
+      <c r="C36" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D36" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="E36" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="F36" s="28">
+        <v>3</v>
+      </c>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="I36" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="J36" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="K36" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="L36" s="14">
+        <v>1</v>
+      </c>
+      <c r="O36" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D37" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="E37" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="F37" s="28">
+        <v>4</v>
+      </c>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="I37" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="J37" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="K37" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="L37" s="14">
+        <v>1</v>
+      </c>
+      <c r="O37" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B38" s="13"/>
+      <c r="C38" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D38" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="E38" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="F38" s="28">
+        <v>5</v>
+      </c>
+      <c r="G38" s="28"/>
+      <c r="H38" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="I38" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="J38" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="K38" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="L38" s="14">
+        <v>1</v>
+      </c>
+      <c r="O38" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B39" s="13"/>
+      <c r="C39" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D39" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="E39" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F39" s="28">
+        <v>1</v>
+      </c>
+      <c r="G39" s="28"/>
+      <c r="H39" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="I39" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="J39" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="K39" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="L39" s="14">
+        <v>2</v>
+      </c>
+      <c r="O39" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A21" xr:uid="{00000000-0002-0000-0700-000001000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A39" xr:uid="{00000000-0002-0000-0700-000001000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B21" xr:uid="{00000000-0002-0000-0700-000002000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B39" xr:uid="{00000000-0002-0000-0700-000002000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -5799,10 +7224,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5885,15 +7310,33 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="13">
+        <v>43466</v>
+      </c>
+      <c r="B5" s="26"/>
+      <c r="C5" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="F5" s="21">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F5" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4" xr:uid="{00000000-0002-0000-0800-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A5" xr:uid="{00000000-0002-0000-0800-000002000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B4" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B4:B5" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -5901,12 +7344,18 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{00000000-0002-0000-0800-000003000000}">
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$9</xm:f>
           </x14:formula1>
           <xm:sqref>D4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{3922A2E3-B39F-854D-BF73-EE32348B2F8C}">
+          <x14:formula1>
+            <xm:f>'/Users/sivakanukollu/github/MOJ/ccd-data-store-api/src/aat/resources/[CCD_BEFTA_JURISDICTION4.xlsx]CaseField'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
RDM-6385: Case type name has been changed to 30 chars. Max is 30 chars for this field.
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_BEFTA_JURISDICTION1.xlsx
+++ b/src/aat/resources/CCD_BEFTA_JURISDICTION1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11111"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sivakanukollu/github/MOJ/ccd-data-store-api/src/aat/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/462450/IdeaProjects/ccd-data-store-api/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145D0F59-424F-BD48-AE07-2D8DB5DAA2E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DDF493-3F88-324F-A982-E1DAA41163DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11560" yWindow="-26880" windowWidth="50900" windowHeight="26880" tabRatio="823" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13460" yWindow="-26880" windowWidth="50900" windowHeight="26880" tabRatio="823" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -645,7 +645,7 @@
     <t>Create a case of type CASE_TYPE_WITH_NO_CASES</t>
   </si>
   <si>
-    <t>Case Type With No Cases - Don't Create</t>
+    <t>CT With No Cases -Don't Create</t>
   </si>
 </sst>
 </file>
@@ -3925,7 +3925,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4083,7 +4083,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4567,7 +4567,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4941,7 +4941,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C12"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5149,7 +5149,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD15"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>